<commit_message>
Präsentation update, Film ist nun drin
</commit_message>
<xml_diff>
--- a/Testphase/TestdatenVideo.xlsx
+++ b/Testphase/TestdatenVideo.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phil\git\Fallstudie\Testphase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="17715" windowHeight="5715"/>
   </bookViews>
@@ -138,8 +143,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,11 +202,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -243,7 +256,7 @@
     </a:clrScheme>
     <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,9 +288,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -309,6 +323,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -484,14 +499,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
@@ -499,12 +514,12 @@
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -515,7 +530,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -526,12 +541,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -545,7 +560,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -559,12 +574,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -584,7 +599,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -604,12 +619,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
@@ -617,7 +632,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -625,48 +640,48 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>18</v>
       </c>
@@ -674,7 +689,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -682,12 +697,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>4</v>
       </c>
@@ -695,7 +710,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -703,10 +718,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
   </sheetData>
@@ -716,24 +731,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
@ralf und update TestdatenVideo
</commit_message>
<xml_diff>
--- a/Testphase/TestdatenVideo.xlsx
+++ b/Testphase/TestdatenVideo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="17715" windowHeight="5715"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="17715" windowHeight="5715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Phil</author>
+  </authors>
+  <commentList>
+    <comment ref="D20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Phil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+3 Arbeitsgruppen ohne Leiter.
+3 Bereiche ohne Leiter.
+Pro AG: 30 Einträge, 5 je Art.
+60 Mitarbeter, 20 je Arbeitsgruppe.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
   <si>
     <t>Arbeitsgruppe anlegen</t>
   </si>
@@ -95,15 +133,9 @@
     <t>Sachbearbeiter</t>
   </si>
   <si>
-    <t>GT</t>
-  </si>
-  <si>
     <t>Karl Becker</t>
   </si>
   <si>
-    <t>Heinz Raubach</t>
-  </si>
-  <si>
     <t>IS</t>
   </si>
   <si>
@@ -138,13 +170,136 @@
   </si>
   <si>
     <t>Suchbegriff</t>
+  </si>
+  <si>
+    <t>Timo Scholl</t>
+  </si>
+  <si>
+    <t>Arbeitsgruppe</t>
+  </si>
+  <si>
+    <t>Timo</t>
+  </si>
+  <si>
+    <t>Scholl</t>
+  </si>
+  <si>
+    <t>Ts</t>
+  </si>
+  <si>
+    <t>Ts1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sachbearbeiter </t>
+  </si>
+  <si>
+    <t>IT-Sicherheit</t>
+  </si>
+  <si>
+    <t>Mitarbeiter</t>
+  </si>
+  <si>
+    <t>Rollenwechsel:</t>
+  </si>
+  <si>
+    <t>Arbeitsgruppe "UHD" wird Leiter = Timo Scholl gesetzt</t>
+  </si>
+  <si>
+    <t>Bereich IS wird Leiter = Timo Scholl gesetzt</t>
+  </si>
+  <si>
+    <t>Zentralbereichsleiter</t>
+  </si>
+  <si>
+    <t>DUMMY EINTRÄGE WERDEN EINGESPIELT</t>
+  </si>
+  <si>
+    <t>ERFASSEN VON EINTRÄGEN</t>
+  </si>
+  <si>
+    <t>JOB LAUFEN LASSEN</t>
+  </si>
+  <si>
+    <t>1.Bereich anlegen</t>
+  </si>
+  <si>
+    <t>2. Arbeitsgruppe anlegen</t>
+  </si>
+  <si>
+    <t>3. Mitarbeiter anlegen</t>
+  </si>
+  <si>
+    <t>3.2 ausloggen</t>
+  </si>
+  <si>
+    <t>Fachbereichsorganisation: admin/admin</t>
+  </si>
+  <si>
+    <t>Einloggen: admin/admin</t>
+  </si>
+  <si>
+    <t>4. Einloggen: admin/admin</t>
+  </si>
+  <si>
+    <t>4.2 Arbeitsgruppe bearbeiten= UHD, Leiter= Scholl</t>
+  </si>
+  <si>
+    <t>5. Einloggen: Ts/Ts1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.1 Daten anzeigen </t>
+  </si>
+  <si>
+    <t>5.2 PDF</t>
+  </si>
+  <si>
+    <t>5.3 CSV + Diagramm erstellen</t>
+  </si>
+  <si>
+    <t>3.1 Einträge erfassen - Arten Zeigen</t>
+  </si>
+  <si>
+    <t>6. Einloggen: admin/admin</t>
+  </si>
+  <si>
+    <t>6.2 Bereich bearbeiten=IS, Leiter=Scholl</t>
+  </si>
+  <si>
+    <t>6.1 Mitarbeiter bearbeiten: Scholl, Rolle= Bereichsleiter</t>
+  </si>
+  <si>
+    <t>4.1 Mitarbeiter bearbeiten: Scholl, Rolle=Gruppenleiter</t>
+  </si>
+  <si>
+    <t>6.3 Dummy Einträge zur Übersicht</t>
+  </si>
+  <si>
+    <t>7. Einloggen: admin/admin</t>
+  </si>
+  <si>
+    <t>7.1 Mitarbeiter bearbeiten: nach IS suchen, Rolle= ZBL</t>
+  </si>
+  <si>
+    <t>7.2 Einträge einsehen</t>
+  </si>
+  <si>
+    <t>7.3 Drill-Down auf Bereichssicht</t>
+  </si>
+  <si>
+    <t>7.4 PDF+CSV</t>
+  </si>
+  <si>
+    <t>8. Einloggen: admin/admin</t>
+  </si>
+  <si>
+    <t>8.1 Mitarbeiter löschen:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,16 +323,78 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -185,20 +402,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Berechnung" xfId="3" builtinId="22"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Überschrift 3" xfId="2" builtinId="18"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="4" builtinId="24"/>
+    <cellStyle name="Warnender Text" xfId="5" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -502,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,13 +830,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -562,16 +860,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -596,7 +894,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -616,17 +914,17 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>17</v>
@@ -634,10 +932,10 @@
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -655,7 +953,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -673,7 +971,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -686,15 +984,15 @@
         <v>18</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -707,15 +1005,15 @@
         <v>4</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -731,14 +1029,289 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
a, pdf test klasse @angelos
</commit_message>
<xml_diff>
--- a/Testphase/TestdatenVideo.xlsx
+++ b/Testphase/TestdatenVideo.xlsx
@@ -466,17 +466,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -489,6 +480,15 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Berechnung" xfId="3" builtinId="22"/>
@@ -1032,13 +1032,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
@@ -1049,11 +1049,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
       <c r="F1" t="s">
         <v>57</v>
       </c>
@@ -1078,11 +1078,11 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -1104,11 +1104,11 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -1152,64 +1152,64 @@
       <c r="F9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="10" t="s">
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="9" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1244,7 +1244,7 @@
       <c r="C18" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1252,7 +1252,7 @@
       <c r="A19" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C19" t="s">
@@ -1272,7 +1272,7 @@
       <c r="C20" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="11" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
       <c r="B21" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="10" t="s">
         <v>73</v>
       </c>
       <c r="D21" t="s">

</xml_diff>